<commit_message>
nsc schedule function, swaps to avoid rematches
</commit_message>
<xml_diff>
--- a/data input/prelims_data.xlsx
+++ b/data input/prelims_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/victorprieto/Desktop/code/cornerstone/data input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A577DDF-D3E0-9B43-B915-3006179617AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{314DDFA0-13DD-0344-9D1C-53911C00C349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="2" xr2:uid="{2114AE23-4723-3F48-88AE-F53CC59B0CBE}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="235">
   <si>
     <t>Team</t>
   </si>
@@ -162,57 +162,12 @@
     <t>Rosemont, IL</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>Enter "Y" or "N" for QR codes to be included.</t>
   </si>
   <si>
     <t>Enter "Y" or "N" for text input to be included.</t>
   </si>
   <si>
-    <t>Saturday, June 12, 2022</t>
-  </si>
-  <si>
-    <t>Link 1</t>
-  </si>
-  <si>
-    <t>none</t>
-  </si>
-  <si>
-    <t>Link 2</t>
-  </si>
-  <si>
-    <t>Link 3</t>
-  </si>
-  <si>
-    <t>Link 4</t>
-  </si>
-  <si>
-    <t>Link 5</t>
-  </si>
-  <si>
-    <t>Link 6</t>
-  </si>
-  <si>
-    <t>This is the placeholder text for the prelim schedule individualized for each team. Useful pieces of information to include in this section are: expected start time and length of time for lunch, information on tiebreakers, where to report back after lunch...</t>
-  </si>
-  <si>
-    <t>This is the placeholder text for the prelim schedule individualized for each room. Useful pieces of information to include in this section are: how to report protests, tiebreaker procedure, where to go for lunch…</t>
-  </si>
-  <si>
-    <t>Group A</t>
-  </si>
-  <si>
-    <t>Group B</t>
-  </si>
-  <si>
-    <t>Group C</t>
-  </si>
-  <si>
-    <t>Group D</t>
-  </si>
-  <si>
     <t>Room 1</t>
   </si>
   <si>
@@ -391,6 +346,426 @@
   </si>
   <si>
     <t>TD6</t>
+  </si>
+  <si>
+    <t>Avenue</t>
+  </si>
+  <si>
+    <t>Bayou</t>
+  </si>
+  <si>
+    <t>Circle</t>
+  </si>
+  <si>
+    <t>Drive</t>
+  </si>
+  <si>
+    <t>Expressway</t>
+  </si>
+  <si>
+    <t>Ford</t>
+  </si>
+  <si>
+    <t>Glen</t>
+  </si>
+  <si>
+    <t>Harbor</t>
+  </si>
+  <si>
+    <t>Inlet</t>
+  </si>
+  <si>
+    <t>Team E1</t>
+  </si>
+  <si>
+    <t>Team E2</t>
+  </si>
+  <si>
+    <t>Team E3</t>
+  </si>
+  <si>
+    <t>Team E4</t>
+  </si>
+  <si>
+    <t>Team E5</t>
+  </si>
+  <si>
+    <t>Team E6</t>
+  </si>
+  <si>
+    <t>Team F1</t>
+  </si>
+  <si>
+    <t>Team F2</t>
+  </si>
+  <si>
+    <t>Team F3</t>
+  </si>
+  <si>
+    <t>Team F4</t>
+  </si>
+  <si>
+    <t>Team F5</t>
+  </si>
+  <si>
+    <t>Team F6</t>
+  </si>
+  <si>
+    <t>Team G1</t>
+  </si>
+  <si>
+    <t>Team G2</t>
+  </si>
+  <si>
+    <t>Team G3</t>
+  </si>
+  <si>
+    <t>Team G4</t>
+  </si>
+  <si>
+    <t>Team G5</t>
+  </si>
+  <si>
+    <t>Team G6</t>
+  </si>
+  <si>
+    <t>Team H1</t>
+  </si>
+  <si>
+    <t>Team H2</t>
+  </si>
+  <si>
+    <t>Team H3</t>
+  </si>
+  <si>
+    <t>Team H4</t>
+  </si>
+  <si>
+    <t>Team H5</t>
+  </si>
+  <si>
+    <t>Team H6</t>
+  </si>
+  <si>
+    <t>Team J1</t>
+  </si>
+  <si>
+    <t>Team J2</t>
+  </si>
+  <si>
+    <t>Team J3</t>
+  </si>
+  <si>
+    <t>Team J4</t>
+  </si>
+  <si>
+    <t>Team J5</t>
+  </si>
+  <si>
+    <t>Team J6</t>
+  </si>
+  <si>
+    <t>Team I1</t>
+  </si>
+  <si>
+    <t>Team I2</t>
+  </si>
+  <si>
+    <t>Team I3</t>
+  </si>
+  <si>
+    <t>Team I4</t>
+  </si>
+  <si>
+    <t>Team I5</t>
+  </si>
+  <si>
+    <t>Team I6</t>
+  </si>
+  <si>
+    <t>Team K1</t>
+  </si>
+  <si>
+    <t>Team K2</t>
+  </si>
+  <si>
+    <t>Team K3</t>
+  </si>
+  <si>
+    <t>Team K4</t>
+  </si>
+  <si>
+    <t>Team K5</t>
+  </si>
+  <si>
+    <t>Team K6</t>
+  </si>
+  <si>
+    <t>Team L1</t>
+  </si>
+  <si>
+    <t>Team L2</t>
+  </si>
+  <si>
+    <t>Team L3</t>
+  </si>
+  <si>
+    <t>Team L4</t>
+  </si>
+  <si>
+    <t>Team L5</t>
+  </si>
+  <si>
+    <t>Team L6</t>
+  </si>
+  <si>
+    <t>Room 13</t>
+  </si>
+  <si>
+    <t>Room 14</t>
+  </si>
+  <si>
+    <t>Room 15</t>
+  </si>
+  <si>
+    <t>Room 16</t>
+  </si>
+  <si>
+    <t>Room 17</t>
+  </si>
+  <si>
+    <t>Room 18</t>
+  </si>
+  <si>
+    <t>Room 19</t>
+  </si>
+  <si>
+    <t>Room 20</t>
+  </si>
+  <si>
+    <t>Room 21</t>
+  </si>
+  <si>
+    <t>Room 22</t>
+  </si>
+  <si>
+    <t>Room 23</t>
+  </si>
+  <si>
+    <t>Room 24</t>
+  </si>
+  <si>
+    <t>Room 25</t>
+  </si>
+  <si>
+    <t>Room 26</t>
+  </si>
+  <si>
+    <t>Room 27</t>
+  </si>
+  <si>
+    <t>Room 28</t>
+  </si>
+  <si>
+    <t>Room 29</t>
+  </si>
+  <si>
+    <t>Room 30</t>
+  </si>
+  <si>
+    <t>Room 31</t>
+  </si>
+  <si>
+    <t>Room 32</t>
+  </si>
+  <si>
+    <t>Room 33</t>
+  </si>
+  <si>
+    <t>Room 34</t>
+  </si>
+  <si>
+    <t>Room 35</t>
+  </si>
+  <si>
+    <t>Room 36</t>
+  </si>
+  <si>
+    <t>TE1</t>
+  </si>
+  <si>
+    <t>TE2</t>
+  </si>
+  <si>
+    <t>TE3</t>
+  </si>
+  <si>
+    <t>TE4</t>
+  </si>
+  <si>
+    <t>TE5</t>
+  </si>
+  <si>
+    <t>TE6</t>
+  </si>
+  <si>
+    <t>TF1</t>
+  </si>
+  <si>
+    <t>TF2</t>
+  </si>
+  <si>
+    <t>TF3</t>
+  </si>
+  <si>
+    <t>TF4</t>
+  </si>
+  <si>
+    <t>TF5</t>
+  </si>
+  <si>
+    <t>TF6</t>
+  </si>
+  <si>
+    <t>TG1</t>
+  </si>
+  <si>
+    <t>TG2</t>
+  </si>
+  <si>
+    <t>TG3</t>
+  </si>
+  <si>
+    <t>TG4</t>
+  </si>
+  <si>
+    <t>TG5</t>
+  </si>
+  <si>
+    <t>TG6</t>
+  </si>
+  <si>
+    <t>TH1</t>
+  </si>
+  <si>
+    <t>TH2</t>
+  </si>
+  <si>
+    <t>TH3</t>
+  </si>
+  <si>
+    <t>TH4</t>
+  </si>
+  <si>
+    <t>TH5</t>
+  </si>
+  <si>
+    <t>TH6</t>
+  </si>
+  <si>
+    <t>TJ1</t>
+  </si>
+  <si>
+    <t>TJ2</t>
+  </si>
+  <si>
+    <t>TJ3</t>
+  </si>
+  <si>
+    <t>TJ4</t>
+  </si>
+  <si>
+    <t>TJ5</t>
+  </si>
+  <si>
+    <t>TJ6</t>
+  </si>
+  <si>
+    <t>Junction</t>
+  </si>
+  <si>
+    <t>Knoll</t>
+  </si>
+  <si>
+    <t>Landing</t>
+  </si>
+  <si>
+    <t>https://forms.gle/AnX5uc7Lu2GpdiwMA</t>
+  </si>
+  <si>
+    <t>Moderator Feedback</t>
+  </si>
+  <si>
+    <t>https://pacensc.github.io/</t>
+  </si>
+  <si>
+    <t>placeholder</t>
+  </si>
+  <si>
+    <t>https://www.hsquizbowl.org/db/</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>This is the placeholder text for the prelim schedule individualized for each team. This is how you create \textbf{bold text} or \textit{italicized text}. Useful pieces of information to include in this section are: expected start time and length of time for lunch, information on tiebreakers, where to report back after lunch...</t>
+  </si>
+  <si>
+    <t>This is the placeholder text for the prelim schedule individualized for each room. This is how you create \textbf{bold text} or \textit{italicized text}. Useful pieces of information to include in this section are: how to report protests, tiebreaker procedure, where to go for lunch…</t>
+  </si>
+  <si>
+    <t>TI1</t>
+  </si>
+  <si>
+    <t>TI2</t>
+  </si>
+  <si>
+    <t>TI3</t>
+  </si>
+  <si>
+    <t>TI4</t>
+  </si>
+  <si>
+    <t>TI5</t>
+  </si>
+  <si>
+    <t>TI6</t>
+  </si>
+  <si>
+    <t>TK1</t>
+  </si>
+  <si>
+    <t>TK2</t>
+  </si>
+  <si>
+    <t>TK3</t>
+  </si>
+  <si>
+    <t>TK4</t>
+  </si>
+  <si>
+    <t>TK5</t>
+  </si>
+  <si>
+    <t>TK6</t>
+  </si>
+  <si>
+    <t>TL1</t>
+  </si>
+  <si>
+    <t>TL2</t>
+  </si>
+  <si>
+    <t>TL3</t>
+  </si>
+  <si>
+    <t>TL4</t>
+  </si>
+  <si>
+    <t>TL5</t>
+  </si>
+  <si>
+    <t>TL6</t>
   </si>
 </sst>
 </file>
@@ -516,7 +891,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -593,6 +968,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -601,7 +989,7 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -622,9 +1010,6 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -632,9 +1017,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
@@ -646,14 +1028,29 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -976,7 +1373,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20"/>
@@ -998,58 +1395,58 @@
       </c>
     </row>
     <row r="2" spans="1:3" s="2" customFormat="1" ht="40" customHeight="1">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="2" customFormat="1" ht="40" customHeight="1">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="2" customFormat="1" ht="40" customHeight="1">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="11" t="s">
+      <c r="B4" s="20">
+        <v>44723</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="2" customFormat="1" ht="40" customHeight="1">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="C5" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="15" t="s">
+    </row>
+    <row r="6" spans="1:3" s="2" customFormat="1" ht="40" customHeight="1">
+      <c r="A6" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="C6" s="13" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" s="2" customFormat="1" ht="40" customHeight="1">
-      <c r="A6" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1070,7 +1467,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D0CB595-5535-8C4C-9710-F68F5657C36B}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C73"/>
   <sheetViews>
     <sheetView zoomScale="119" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1080,8 +1477,8 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20"/>
   <cols>
     <col min="1" max="1" width="28.109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="10.77734375" style="3"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" ht="30" customHeight="1">
@@ -1096,290 +1493,866 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="13" t="s">
-        <v>62</v>
+      <c r="A2" s="11" t="s">
+        <v>47</v>
       </c>
       <c r="B2" s="4" t="str">
         <f>'group names'!A$2</f>
-        <v>Group A</v>
+        <v>Avenue</v>
       </c>
       <c r="C2" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="13" t="s">
-        <v>64</v>
+      <c r="A3" s="11" t="s">
+        <v>49</v>
       </c>
       <c r="B3" s="4" t="str">
         <f>'group names'!A$2</f>
-        <v>Group A</v>
+        <v>Avenue</v>
       </c>
       <c r="C3" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="13" t="s">
-        <v>66</v>
+      <c r="A4" s="11" t="s">
+        <v>51</v>
       </c>
       <c r="B4" s="4" t="str">
         <f>'group names'!A$2</f>
-        <v>Group A</v>
+        <v>Avenue</v>
       </c>
       <c r="C4" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="13" t="s">
-        <v>68</v>
+      <c r="A5" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="B5" s="4" t="str">
         <f>'group names'!A$2</f>
-        <v>Group A</v>
+        <v>Avenue</v>
       </c>
       <c r="C5" s="4">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="13" t="s">
-        <v>70</v>
+      <c r="A6" s="11" t="s">
+        <v>55</v>
       </c>
       <c r="B6" s="4" t="str">
         <f>'group names'!A$2</f>
-        <v>Group A</v>
+        <v>Avenue</v>
       </c>
       <c r="C6" s="4">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="13" t="s">
-        <v>72</v>
+      <c r="A7" s="11" t="s">
+        <v>57</v>
       </c>
       <c r="B7" s="4" t="str">
         <f>'group names'!A$2</f>
-        <v>Group A</v>
+        <v>Avenue</v>
       </c>
       <c r="C7" s="4">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="13" t="s">
-        <v>74</v>
+      <c r="A8" s="11" t="s">
+        <v>59</v>
       </c>
       <c r="B8" s="4" t="str">
         <f>'group names'!A$3</f>
-        <v>Group B</v>
+        <v>Bayou</v>
       </c>
       <c r="C8" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="13" t="s">
-        <v>76</v>
+      <c r="A9" s="11" t="s">
+        <v>61</v>
       </c>
       <c r="B9" s="4" t="str">
         <f>'group names'!A$3</f>
-        <v>Group B</v>
+        <v>Bayou</v>
       </c>
       <c r="C9" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="13" t="s">
-        <v>78</v>
+      <c r="A10" s="11" t="s">
+        <v>63</v>
       </c>
       <c r="B10" s="4" t="str">
         <f>'group names'!A$3</f>
-        <v>Group B</v>
+        <v>Bayou</v>
       </c>
       <c r="C10" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="13" t="s">
-        <v>80</v>
+      <c r="A11" s="11" t="s">
+        <v>65</v>
       </c>
       <c r="B11" s="4" t="str">
         <f>'group names'!A$3</f>
-        <v>Group B</v>
+        <v>Bayou</v>
       </c>
       <c r="C11" s="4">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="13" t="s">
-        <v>82</v>
+      <c r="A12" s="11" t="s">
+        <v>67</v>
       </c>
       <c r="B12" s="4" t="str">
         <f>'group names'!A$3</f>
-        <v>Group B</v>
+        <v>Bayou</v>
       </c>
       <c r="C12" s="4">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="13" t="s">
-        <v>84</v>
+      <c r="A13" s="11" t="s">
+        <v>69</v>
       </c>
       <c r="B13" s="4" t="str">
         <f>'group names'!A$3</f>
-        <v>Group B</v>
+        <v>Bayou</v>
       </c>
       <c r="C13" s="4">
         <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="13" t="s">
-        <v>86</v>
+      <c r="A14" s="11" t="s">
+        <v>71</v>
       </c>
       <c r="B14" s="4" t="str">
         <f>'group names'!A$4</f>
-        <v>Group C</v>
+        <v>Circle</v>
       </c>
       <c r="C14" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="13" t="s">
-        <v>88</v>
+      <c r="A15" s="11" t="s">
+        <v>73</v>
       </c>
       <c r="B15" s="4" t="str">
         <f>'group names'!A$4</f>
-        <v>Group C</v>
+        <v>Circle</v>
       </c>
       <c r="C15" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="13" t="s">
-        <v>90</v>
+      <c r="A16" s="11" t="s">
+        <v>75</v>
       </c>
       <c r="B16" s="4" t="str">
         <f>'group names'!A$4</f>
-        <v>Group C</v>
+        <v>Circle</v>
       </c>
       <c r="C16" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="13" t="s">
-        <v>92</v>
+      <c r="A17" s="11" t="s">
+        <v>77</v>
       </c>
       <c r="B17" s="4" t="str">
         <f>'group names'!A$4</f>
-        <v>Group C</v>
+        <v>Circle</v>
       </c>
       <c r="C17" s="4">
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="13" t="s">
-        <v>94</v>
+      <c r="A18" s="11" t="s">
+        <v>79</v>
       </c>
       <c r="B18" s="4" t="str">
         <f>'group names'!A$4</f>
-        <v>Group C</v>
+        <v>Circle</v>
       </c>
       <c r="C18" s="4">
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="13" t="s">
-        <v>96</v>
+      <c r="A19" s="11" t="s">
+        <v>81</v>
       </c>
       <c r="B19" s="4" t="str">
         <f>'group names'!A$4</f>
-        <v>Group C</v>
+        <v>Circle</v>
       </c>
       <c r="C19" s="4">
         <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="13" t="s">
-        <v>98</v>
+      <c r="A20" s="11" t="s">
+        <v>83</v>
       </c>
       <c r="B20" s="4" t="str">
         <f>'group names'!A$5</f>
-        <v>Group D</v>
+        <v>Drive</v>
       </c>
       <c r="C20" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="13" t="s">
-        <v>100</v>
+      <c r="A21" s="11" t="s">
+        <v>85</v>
       </c>
       <c r="B21" s="4" t="str">
         <f>'group names'!A$5</f>
-        <v>Group D</v>
+        <v>Drive</v>
       </c>
       <c r="C21" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="13" t="s">
-        <v>102</v>
+      <c r="A22" s="11" t="s">
+        <v>87</v>
       </c>
       <c r="B22" s="4" t="str">
         <f>'group names'!A$5</f>
-        <v>Group D</v>
+        <v>Drive</v>
       </c>
       <c r="C22" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="13" t="s">
-        <v>104</v>
+      <c r="A23" s="11" t="s">
+        <v>89</v>
       </c>
       <c r="B23" s="4" t="str">
         <f>'group names'!A$5</f>
-        <v>Group D</v>
+        <v>Drive</v>
       </c>
       <c r="C23" s="4">
         <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="13" t="s">
-        <v>106</v>
+      <c r="A24" s="11" t="s">
+        <v>91</v>
       </c>
       <c r="B24" s="4" t="str">
         <f>'group names'!A$5</f>
-        <v>Group D</v>
+        <v>Drive</v>
       </c>
       <c r="C24" s="4">
         <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="13" t="s">
-        <v>108</v>
+      <c r="A25" s="11" t="s">
+        <v>93</v>
       </c>
       <c r="B25" s="4" t="str">
         <f>'group names'!A$5</f>
-        <v>Group D</v>
+        <v>Drive</v>
       </c>
       <c r="C25" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="B26" s="4" t="str">
+        <f>'group names'!A$6</f>
+        <v>Expressway</v>
+      </c>
+      <c r="C26" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="B27" s="4" t="str">
+        <f>'group names'!A$6</f>
+        <v>Expressway</v>
+      </c>
+      <c r="C27" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="B28" s="4" t="str">
+        <f>'group names'!A$6</f>
+        <v>Expressway</v>
+      </c>
+      <c r="C28" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B29" s="4" t="str">
+        <f>'group names'!A$6</f>
+        <v>Expressway</v>
+      </c>
+      <c r="C29" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B30" s="4" t="str">
+        <f>'group names'!A$6</f>
+        <v>Expressway</v>
+      </c>
+      <c r="C30" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="B31" s="4" t="str">
+        <f>'group names'!A$6</f>
+        <v>Expressway</v>
+      </c>
+      <c r="C31" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="B32" s="4" t="str">
+        <f>'group names'!A$7</f>
+        <v>Ford</v>
+      </c>
+      <c r="C32" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="B33" s="4" t="str">
+        <f>'group names'!A$7</f>
+        <v>Ford</v>
+      </c>
+      <c r="C33" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="B34" s="4" t="str">
+        <f>'group names'!A$7</f>
+        <v>Ford</v>
+      </c>
+      <c r="C34" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="B35" s="4" t="str">
+        <f>'group names'!A$7</f>
+        <v>Ford</v>
+      </c>
+      <c r="C35" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B36" s="4" t="str">
+        <f>'group names'!A$7</f>
+        <v>Ford</v>
+      </c>
+      <c r="C36" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="B37" s="4" t="str">
+        <f>'group names'!A$7</f>
+        <v>Ford</v>
+      </c>
+      <c r="C37" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="B38" s="4" t="str">
+        <f>'group names'!A$8</f>
+        <v>Glen</v>
+      </c>
+      <c r="C38" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="B39" s="4" t="str">
+        <f>'group names'!A$8</f>
+        <v>Glen</v>
+      </c>
+      <c r="C39" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="B40" s="4" t="str">
+        <f>'group names'!A$8</f>
+        <v>Glen</v>
+      </c>
+      <c r="C40" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="B41" s="4" t="str">
+        <f>'group names'!A$8</f>
+        <v>Glen</v>
+      </c>
+      <c r="C41" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="B42" s="4" t="str">
+        <f>'group names'!A$8</f>
+        <v>Glen</v>
+      </c>
+      <c r="C42" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="B43" s="4" t="str">
+        <f>'group names'!A$8</f>
+        <v>Glen</v>
+      </c>
+      <c r="C43" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="B44" s="4" t="str">
+        <f>'group names'!A$9</f>
+        <v>Harbor</v>
+      </c>
+      <c r="C44" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="B45" s="4" t="str">
+        <f>'group names'!A$9</f>
+        <v>Harbor</v>
+      </c>
+      <c r="C45" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B46" s="4" t="str">
+        <f>'group names'!A$9</f>
+        <v>Harbor</v>
+      </c>
+      <c r="C46" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="B47" s="4" t="str">
+        <f>'group names'!A$9</f>
+        <v>Harbor</v>
+      </c>
+      <c r="C47" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B48" s="4" t="str">
+        <f>'group names'!A$9</f>
+        <v>Harbor</v>
+      </c>
+      <c r="C48" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="B49" s="4" t="str">
+        <f>'group names'!A$9</f>
+        <v>Harbor</v>
+      </c>
+      <c r="C49" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B50" s="4" t="str">
+        <f>'group names'!A$10</f>
+        <v>Inlet</v>
+      </c>
+      <c r="C50" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="B51" s="4" t="str">
+        <f>'group names'!A$10</f>
+        <v>Inlet</v>
+      </c>
+      <c r="C51" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="B52" s="4" t="str">
+        <f>'group names'!A$10</f>
+        <v>Inlet</v>
+      </c>
+      <c r="C52" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B53" s="4" t="str">
+        <f>'group names'!A$10</f>
+        <v>Inlet</v>
+      </c>
+      <c r="C53" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="B54" s="4" t="str">
+        <f>'group names'!A$10</f>
+        <v>Inlet</v>
+      </c>
+      <c r="C54" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B55" s="4" t="str">
+        <f>'group names'!A$10</f>
+        <v>Inlet</v>
+      </c>
+      <c r="C55" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="B56" s="4" t="str">
+        <f>'group names'!A$11</f>
+        <v>Junction</v>
+      </c>
+      <c r="C56" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B57" s="4" t="str">
+        <f>'group names'!A$11</f>
+        <v>Junction</v>
+      </c>
+      <c r="C57" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="B58" s="4" t="str">
+        <f>'group names'!A$11</f>
+        <v>Junction</v>
+      </c>
+      <c r="C58" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="B59" s="4" t="str">
+        <f>'group names'!A$11</f>
+        <v>Junction</v>
+      </c>
+      <c r="C59" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="B60" s="4" t="str">
+        <f>'group names'!A$11</f>
+        <v>Junction</v>
+      </c>
+      <c r="C60" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="B61" s="4" t="str">
+        <f>'group names'!A$11</f>
+        <v>Junction</v>
+      </c>
+      <c r="C61" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="B62" s="4" t="str">
+        <f>'group names'!A$12</f>
+        <v>Knoll</v>
+      </c>
+      <c r="C62" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B63" s="4" t="str">
+        <f>'group names'!A$12</f>
+        <v>Knoll</v>
+      </c>
+      <c r="C63" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="B64" s="4" t="str">
+        <f>'group names'!A$12</f>
+        <v>Knoll</v>
+      </c>
+      <c r="C64" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="B65" s="4" t="str">
+        <f>'group names'!A$12</f>
+        <v>Knoll</v>
+      </c>
+      <c r="C65" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="B66" s="4" t="str">
+        <f>'group names'!A$12</f>
+        <v>Knoll</v>
+      </c>
+      <c r="C66" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="B67" s="4" t="str">
+        <f>'group names'!A$12</f>
+        <v>Knoll</v>
+      </c>
+      <c r="C67" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="B68" s="4" t="str">
+        <f>'group names'!A$13</f>
+        <v>Landing</v>
+      </c>
+      <c r="C68" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="B69" s="4" t="str">
+        <f>'group names'!A$13</f>
+        <v>Landing</v>
+      </c>
+      <c r="C69" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="B70" s="4" t="str">
+        <f>'group names'!A$13</f>
+        <v>Landing</v>
+      </c>
+      <c r="C70" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="B71" s="4" t="str">
+        <f>'group names'!A$13</f>
+        <v>Landing</v>
+      </c>
+      <c r="C71" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="B72" s="4" t="str">
+        <f>'group names'!A$13</f>
+        <v>Landing</v>
+      </c>
+      <c r="C72" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="B73" s="4" t="str">
+        <f>'group names'!A$13</f>
+        <v>Landing</v>
+      </c>
+      <c r="C73" s="4">
         <v>6</v>
       </c>
     </row>
@@ -1392,9 +2365,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7094DA6C-F5D8-904A-9463-23A0D10AE5DA}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="173" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="173" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
   <cols>
@@ -1403,227 +2378,659 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="16" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="5" t="str">
+      <c r="A2" s="17" t="str">
         <f>'list of teams'!A2</f>
         <v>Team A1</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>63</v>
+      <c r="B2" s="11" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="5" t="str">
+      <c r="A3" s="17" t="str">
         <f>'list of teams'!A3</f>
         <v>Team A2</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>65</v>
+      <c r="B3" s="11" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="5" t="str">
+      <c r="A4" s="17" t="str">
         <f>'list of teams'!A4</f>
         <v>Team A3</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>67</v>
+      <c r="B4" s="11" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="5" t="str">
+      <c r="A5" s="17" t="str">
         <f>'list of teams'!A5</f>
         <v>Team A4</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>69</v>
+      <c r="B5" s="11" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="5" t="str">
+      <c r="A6" s="17" t="str">
         <f>'list of teams'!A6</f>
         <v>Team A5</v>
       </c>
-      <c r="B6" s="13" t="s">
-        <v>71</v>
+      <c r="B6" s="11" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="5" t="str">
+      <c r="A7" s="17" t="str">
         <f>'list of teams'!A7</f>
         <v>Team A6</v>
       </c>
-      <c r="B7" s="13" t="s">
-        <v>73</v>
+      <c r="B7" s="11" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="5" t="str">
+      <c r="A8" s="17" t="str">
         <f>'list of teams'!A8</f>
         <v>Team B1</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>75</v>
+      <c r="B8" s="11" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="5" t="str">
+      <c r="A9" s="17" t="str">
         <f>'list of teams'!A9</f>
         <v>Team B2</v>
       </c>
-      <c r="B9" s="13" t="s">
-        <v>77</v>
+      <c r="B9" s="11" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="5" t="str">
+      <c r="A10" s="17" t="str">
         <f>'list of teams'!A10</f>
         <v>Team B3</v>
       </c>
-      <c r="B10" s="13" t="s">
-        <v>79</v>
+      <c r="B10" s="11" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="5" t="str">
+      <c r="A11" s="17" t="str">
         <f>'list of teams'!A11</f>
         <v>Team B4</v>
       </c>
-      <c r="B11" s="13" t="s">
-        <v>81</v>
+      <c r="B11" s="11" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="5" t="str">
+      <c r="A12" s="17" t="str">
         <f>'list of teams'!A12</f>
         <v>Team B5</v>
       </c>
-      <c r="B12" s="13" t="s">
-        <v>83</v>
+      <c r="B12" s="11" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="5" t="str">
+      <c r="A13" s="17" t="str">
         <f>'list of teams'!A13</f>
         <v>Team B6</v>
       </c>
-      <c r="B13" s="13" t="s">
-        <v>85</v>
+      <c r="B13" s="11" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="5" t="str">
+      <c r="A14" s="17" t="str">
         <f>'list of teams'!A14</f>
         <v>Team C1</v>
       </c>
-      <c r="B14" s="13" t="s">
-        <v>87</v>
+      <c r="B14" s="11" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="5" t="str">
+      <c r="A15" s="17" t="str">
         <f>'list of teams'!A15</f>
         <v>Team C2</v>
       </c>
-      <c r="B15" s="13" t="s">
-        <v>89</v>
+      <c r="B15" s="11" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="5" t="str">
+      <c r="A16" s="17" t="str">
         <f>'list of teams'!A16</f>
         <v>Team C3</v>
       </c>
-      <c r="B16" s="13" t="s">
-        <v>91</v>
+      <c r="B16" s="11" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="5" t="str">
+      <c r="A17" s="17" t="str">
         <f>'list of teams'!A17</f>
         <v>Team C4</v>
       </c>
-      <c r="B17" s="13" t="s">
-        <v>93</v>
+      <c r="B17" s="11" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="5" t="str">
+      <c r="A18" s="17" t="str">
         <f>'list of teams'!A18</f>
         <v>Team C5</v>
       </c>
-      <c r="B18" s="13" t="s">
-        <v>95</v>
+      <c r="B18" s="11" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="5" t="str">
+      <c r="A19" s="17" t="str">
         <f>'list of teams'!A19</f>
         <v>Team C6</v>
       </c>
-      <c r="B19" s="13" t="s">
-        <v>97</v>
+      <c r="B19" s="11" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="5" t="str">
+      <c r="A20" s="17" t="str">
         <f>'list of teams'!A20</f>
         <v>Team D1</v>
       </c>
-      <c r="B20" s="13" t="s">
-        <v>99</v>
+      <c r="B20" s="11" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="5" t="str">
+      <c r="A21" s="17" t="str">
         <f>'list of teams'!A21</f>
         <v>Team D2</v>
       </c>
-      <c r="B21" s="13" t="s">
-        <v>101</v>
+      <c r="B21" s="11" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="5" t="str">
+      <c r="A22" s="17" t="str">
         <f>'list of teams'!A22</f>
         <v>Team D3</v>
       </c>
-      <c r="B22" s="13" t="s">
-        <v>103</v>
+      <c r="B22" s="11" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="5" t="str">
+      <c r="A23" s="17" t="str">
         <f>'list of teams'!A23</f>
         <v>Team D4</v>
       </c>
-      <c r="B23" s="13" t="s">
-        <v>105</v>
+      <c r="B23" s="11" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="5" t="str">
+      <c r="A24" s="17" t="str">
         <f>'list of teams'!A24</f>
         <v>Team D5</v>
       </c>
-      <c r="B24" s="13" t="s">
-        <v>107</v>
+      <c r="B24" s="11" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="5" t="str">
+      <c r="A25" s="17" t="str">
         <f>'list of teams'!A25</f>
         <v>Team D6</v>
       </c>
-      <c r="B25" s="13" t="s">
-        <v>109</v>
+      <c r="B25" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="17" t="str">
+        <f>'list of teams'!A26</f>
+        <v>Team E1</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="17" t="str">
+        <f>'list of teams'!A27</f>
+        <v>Team E2</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="17" t="str">
+        <f>'list of teams'!A28</f>
+        <v>Team E3</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="17" t="str">
+        <f>'list of teams'!A29</f>
+        <v>Team E4</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="17" t="str">
+        <f>'list of teams'!A30</f>
+        <v>Team E5</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="17" t="str">
+        <f>'list of teams'!A31</f>
+        <v>Team E6</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="17" t="str">
+        <f>'list of teams'!A32</f>
+        <v>Team F1</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="17" t="str">
+        <f>'list of teams'!A33</f>
+        <v>Team F2</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="17" t="str">
+        <f>'list of teams'!A34</f>
+        <v>Team F3</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="17" t="str">
+        <f>'list of teams'!A35</f>
+        <v>Team F4</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="17" t="str">
+        <f>'list of teams'!A36</f>
+        <v>Team F5</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="17" t="str">
+        <f>'list of teams'!A37</f>
+        <v>Team F6</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="17" t="str">
+        <f>'list of teams'!A38</f>
+        <v>Team G1</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="17" t="str">
+        <f>'list of teams'!A39</f>
+        <v>Team G2</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="17" t="str">
+        <f>'list of teams'!A40</f>
+        <v>Team G3</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="17" t="str">
+        <f>'list of teams'!A41</f>
+        <v>Team G4</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="17" t="str">
+        <f>'list of teams'!A42</f>
+        <v>Team G5</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="17" t="str">
+        <f>'list of teams'!A43</f>
+        <v>Team G6</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="17" t="str">
+        <f>'list of teams'!A44</f>
+        <v>Team H1</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="17" t="str">
+        <f>'list of teams'!A45</f>
+        <v>Team H2</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="17" t="str">
+        <f>'list of teams'!A46</f>
+        <v>Team H3</v>
+      </c>
+      <c r="B46" s="11" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="17" t="str">
+        <f>'list of teams'!A47</f>
+        <v>Team H4</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="17" t="str">
+        <f>'list of teams'!A48</f>
+        <v>Team H5</v>
+      </c>
+      <c r="B48" s="11" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="17" t="str">
+        <f>'list of teams'!A49</f>
+        <v>Team H6</v>
+      </c>
+      <c r="B49" s="11" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="17" t="str">
+        <f>'list of teams'!A50</f>
+        <v>Team I1</v>
+      </c>
+      <c r="B50" s="11" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="17" t="str">
+        <f>'list of teams'!A51</f>
+        <v>Team I2</v>
+      </c>
+      <c r="B51" s="11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="17" t="str">
+        <f>'list of teams'!A52</f>
+        <v>Team I3</v>
+      </c>
+      <c r="B52" s="11" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="17" t="str">
+        <f>'list of teams'!A53</f>
+        <v>Team I4</v>
+      </c>
+      <c r="B53" s="11" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="17" t="str">
+        <f>'list of teams'!A54</f>
+        <v>Team I5</v>
+      </c>
+      <c r="B54" s="11" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="17" t="str">
+        <f>'list of teams'!A55</f>
+        <v>Team I6</v>
+      </c>
+      <c r="B55" s="11" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="17" t="str">
+        <f>'list of teams'!A56</f>
+        <v>Team J1</v>
+      </c>
+      <c r="B56" s="11" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="17" t="str">
+        <f>'list of teams'!A57</f>
+        <v>Team J2</v>
+      </c>
+      <c r="B57" s="11" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="17" t="str">
+        <f>'list of teams'!A58</f>
+        <v>Team J3</v>
+      </c>
+      <c r="B58" s="11" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="17" t="str">
+        <f>'list of teams'!A59</f>
+        <v>Team J4</v>
+      </c>
+      <c r="B59" s="11" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="17" t="str">
+        <f>'list of teams'!A60</f>
+        <v>Team J5</v>
+      </c>
+      <c r="B60" s="11" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="17" t="str">
+        <f>'list of teams'!A61</f>
+        <v>Team J6</v>
+      </c>
+      <c r="B61" s="11" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="17" t="str">
+        <f>'list of teams'!A62</f>
+        <v>Team K1</v>
+      </c>
+      <c r="B62" s="11" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="17" t="str">
+        <f>'list of teams'!A63</f>
+        <v>Team K2</v>
+      </c>
+      <c r="B63" s="11" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="17" t="str">
+        <f>'list of teams'!A64</f>
+        <v>Team K3</v>
+      </c>
+      <c r="B64" s="11" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="17" t="str">
+        <f>'list of teams'!A65</f>
+        <v>Team K4</v>
+      </c>
+      <c r="B65" s="11" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="17" t="str">
+        <f>'list of teams'!A66</f>
+        <v>Team K5</v>
+      </c>
+      <c r="B66" s="11" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="17" t="str">
+        <f>'list of teams'!A67</f>
+        <v>Team K6</v>
+      </c>
+      <c r="B67" s="11" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="17" t="str">
+        <f>'list of teams'!A68</f>
+        <v>Team L1</v>
+      </c>
+      <c r="B68" s="11" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="17" t="str">
+        <f>'list of teams'!A69</f>
+        <v>Team L2</v>
+      </c>
+      <c r="B69" s="11" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="17" t="str">
+        <f>'list of teams'!A70</f>
+        <v>Team L3</v>
+      </c>
+      <c r="B70" s="11" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="17" t="str">
+        <f>'list of teams'!A71</f>
+        <v>Team L4</v>
+      </c>
+      <c r="B71" s="11" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" s="17" t="str">
+        <f>'list of teams'!A72</f>
+        <v>Team L5</v>
+      </c>
+      <c r="B72" s="11" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="17" t="str">
+        <f>'list of teams'!A73</f>
+        <v>Team L6</v>
+      </c>
+      <c r="B73" s="11" t="s">
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -1633,7 +3040,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FF3F05E-06AC-6A4B-A200-208805A45293}">
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView zoomScale="94" zoomScaleNormal="94" workbookViewId="0"/>
   </sheetViews>
@@ -1642,51 +3049,76 @@
     <col min="1" max="1" width="19.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="2" customFormat="1" ht="40" customHeight="1">
+    <row r="1" spans="1:1" s="2" customFormat="1" ht="43" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:1" s="2" customFormat="1" ht="40" customHeight="1">
-      <c r="A2" s="14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" s="2" customFormat="1" ht="40" customHeight="1">
-      <c r="A3" s="14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" s="2" customFormat="1" ht="40" customHeight="1">
-      <c r="A4" s="14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" s="2" customFormat="1" ht="40" customHeight="1">
-      <c r="A5" s="14" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" s="1"/>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="1"/>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" s="1"/>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" s="1"/>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" s="1"/>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" s="1"/>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" s="1"/>
+    <row r="2" spans="1:1" s="2" customFormat="1" ht="43" customHeight="1">
+      <c r="A2" s="12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" s="2" customFormat="1" ht="43" customHeight="1">
+      <c r="A3" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" s="2" customFormat="1" ht="43" customHeight="1">
+      <c r="A4" s="12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" s="2" customFormat="1" ht="43" customHeight="1">
+      <c r="A5" s="12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="43" customHeight="1">
+      <c r="A6" s="12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="43" customHeight="1">
+      <c r="A7" s="12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="43" customHeight="1">
+      <c r="A8" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="43" customHeight="1">
+      <c r="A9" s="12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="43" customHeight="1">
+      <c r="A10" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="43" customHeight="1">
+      <c r="A11" s="9" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="43" customHeight="1">
+      <c r="A12" s="9" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="43" customHeight="1">
+      <c r="A13" s="9" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="1"/>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="1"/>
     </row>
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0"/>
@@ -1698,9 +3130,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B02CA44-6EE3-1E45-A0FA-E7B275D443B3}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20"/>
   <cols>
@@ -1721,146 +3155,434 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="10" t="s">
-        <v>50</v>
+      <c r="A2" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="B2" s="5" t="str">
         <f>'group names'!A$2</f>
-        <v>Group A</v>
+        <v>Avenue</v>
       </c>
       <c r="C2" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="10" t="s">
-        <v>51</v>
+      <c r="A3" s="9" t="s">
+        <v>36</v>
       </c>
       <c r="B3" s="5" t="str">
         <f>'group names'!A$2</f>
-        <v>Group A</v>
+        <v>Avenue</v>
       </c>
       <c r="C3" s="5">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="10" t="s">
-        <v>52</v>
+      <c r="A4" s="9" t="s">
+        <v>37</v>
       </c>
       <c r="B4" s="5" t="str">
         <f>'group names'!A$2</f>
-        <v>Group A</v>
+        <v>Avenue</v>
       </c>
       <c r="C4" s="5">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="10" t="s">
-        <v>53</v>
+      <c r="A5" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="B5" s="5" t="str">
         <f>'group names'!A$3</f>
-        <v>Group B</v>
+        <v>Bayou</v>
       </c>
       <c r="C5" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="10" t="s">
-        <v>54</v>
+      <c r="A6" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="B6" s="5" t="str">
         <f>'group names'!A$3</f>
-        <v>Group B</v>
+        <v>Bayou</v>
       </c>
       <c r="C6" s="5">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="10" t="s">
-        <v>55</v>
+      <c r="A7" s="9" t="s">
+        <v>40</v>
       </c>
       <c r="B7" s="5" t="str">
         <f>'group names'!A$3</f>
-        <v>Group B</v>
+        <v>Bayou</v>
       </c>
       <c r="C7" s="5">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="10" t="s">
-        <v>56</v>
+      <c r="A8" s="9" t="s">
+        <v>41</v>
       </c>
       <c r="B8" s="5" t="str">
         <f>'group names'!A$4</f>
-        <v>Group C</v>
+        <v>Circle</v>
       </c>
       <c r="C8" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="10" t="s">
-        <v>57</v>
+      <c r="A9" s="9" t="s">
+        <v>42</v>
       </c>
       <c r="B9" s="5" t="str">
         <f>'group names'!A$4</f>
-        <v>Group C</v>
+        <v>Circle</v>
       </c>
       <c r="C9" s="5">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="10" t="s">
-        <v>58</v>
+      <c r="A10" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="B10" s="5" t="str">
         <f>'group names'!A$4</f>
-        <v>Group C</v>
+        <v>Circle</v>
       </c>
       <c r="C10" s="5">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="10" t="s">
-        <v>59</v>
+      <c r="A11" s="9" t="s">
+        <v>44</v>
       </c>
       <c r="B11" s="5" t="str">
         <f>'group names'!A$5</f>
-        <v>Group D</v>
+        <v>Drive</v>
       </c>
       <c r="C11" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="10" t="s">
-        <v>60</v>
+      <c r="A12" s="9" t="s">
+        <v>45</v>
       </c>
       <c r="B12" s="5" t="str">
         <f>'group names'!A$5</f>
-        <v>Group D</v>
+        <v>Drive</v>
       </c>
       <c r="C12" s="5">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="10" t="s">
-        <v>61</v>
+      <c r="A13" s="9" t="s">
+        <v>46</v>
       </c>
       <c r="B13" s="5" t="str">
         <f>'group names'!A$5</f>
-        <v>Group D</v>
+        <v>Drive</v>
       </c>
       <c r="C13" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="B14" s="5" t="str">
+        <f>'group names'!A$6</f>
+        <v>Expressway</v>
+      </c>
+      <c r="C14" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="B15" s="5" t="str">
+        <f>'group names'!A$6</f>
+        <v>Expressway</v>
+      </c>
+      <c r="C15" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="B16" s="5" t="str">
+        <f>'group names'!A$6</f>
+        <v>Expressway</v>
+      </c>
+      <c r="C16" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="B17" s="5" t="str">
+        <f>'group names'!A$7</f>
+        <v>Ford</v>
+      </c>
+      <c r="C17" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="B18" s="5" t="str">
+        <f>'group names'!A$7</f>
+        <v>Ford</v>
+      </c>
+      <c r="C18" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="B19" s="5" t="str">
+        <f>'group names'!A$7</f>
+        <v>Ford</v>
+      </c>
+      <c r="C19" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="B20" s="5" t="str">
+        <f>'group names'!A$8</f>
+        <v>Glen</v>
+      </c>
+      <c r="C20" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="B21" s="5" t="str">
+        <f>'group names'!A$8</f>
+        <v>Glen</v>
+      </c>
+      <c r="C21" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="B22" s="5" t="str">
+        <f>'group names'!A$8</f>
+        <v>Glen</v>
+      </c>
+      <c r="C22" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="B23" s="5" t="str">
+        <f>'group names'!A$9</f>
+        <v>Harbor</v>
+      </c>
+      <c r="C23" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="B24" s="5" t="str">
+        <f>'group names'!A$9</f>
+        <v>Harbor</v>
+      </c>
+      <c r="C24" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="B25" s="5" t="str">
+        <f>'group names'!A$9</f>
+        <v>Harbor</v>
+      </c>
+      <c r="C25" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="B26" s="5" t="str">
+        <f>'group names'!A$10</f>
+        <v>Inlet</v>
+      </c>
+      <c r="C26" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="B27" s="5" t="str">
+        <f>'group names'!A$10</f>
+        <v>Inlet</v>
+      </c>
+      <c r="C27" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="B28" s="5" t="str">
+        <f>'group names'!A$10</f>
+        <v>Inlet</v>
+      </c>
+      <c r="C28" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="B29" s="5" t="str">
+        <f>'group names'!A$11</f>
+        <v>Junction</v>
+      </c>
+      <c r="C29" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="B30" s="5" t="str">
+        <f>'group names'!A$11</f>
+        <v>Junction</v>
+      </c>
+      <c r="C30" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="B31" s="5" t="str">
+        <f>'group names'!A$11</f>
+        <v>Junction</v>
+      </c>
+      <c r="C31" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="B32" s="5" t="str">
+        <f>'group names'!A$12</f>
+        <v>Knoll</v>
+      </c>
+      <c r="C32" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="B33" s="5" t="str">
+        <f>'group names'!A$12</f>
+        <v>Knoll</v>
+      </c>
+      <c r="C33" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="B34" s="5" t="str">
+        <f>'group names'!A$12</f>
+        <v>Knoll</v>
+      </c>
+      <c r="C34" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="B35" s="5" t="str">
+        <f>'group names'!A$13</f>
+        <v>Landing</v>
+      </c>
+      <c r="C35" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="B36" s="5" t="str">
+        <f>'group names'!A$13</f>
+        <v>Landing</v>
+      </c>
+      <c r="C36" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="B37" s="5" t="str">
+        <f>'group names'!A$13</f>
+        <v>Landing</v>
+      </c>
+      <c r="C37" s="5">
         <v>3</v>
       </c>
     </row>
@@ -1875,7 +3597,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10058E87-174A-E14F-9AEE-7ACFACE9B5BB}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20"/>
   <cols>
@@ -1892,7 +3616,7 @@
       <c r="B1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="19" t="s">
         <v>25</v>
       </c>
       <c r="D1" s="6" t="s">
@@ -1903,97 +3627,99 @@
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>38</v>
+      <c r="C2" s="21" t="s">
+        <v>209</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>38</v>
+      <c r="C3" s="21" t="s">
+        <v>211</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>38</v>
+      <c r="C4" s="21" t="s">
+        <v>213</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>38</v>
+      <c r="C5" s="21" t="s">
+        <v>209</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>38</v>
+      <c r="C6" s="21" t="s">
+        <v>211</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>38</v>
+      <c r="C7" s="21" t="s">
+        <v>213</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>212</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0"/>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="https://hsquizbowl.org/db/tournaments/7370/" xr:uid="{CB69C4AA-6D2C-2D4F-ACA0-A2ADDE268125}"/>
-    <hyperlink ref="C3" r:id="rId2" display="https://acf-quizbowl.com/gameplay-rules/" xr:uid="{2C94EC85-FE0E-234D-9ABC-633C6F7E638E}"/>
-    <hyperlink ref="C6" r:id="rId3" display="https://acf-quizbowl.com/gameplay-rules/" xr:uid="{E4742F99-FE13-BE49-B8C6-51B35D7A0DCF}"/>
-    <hyperlink ref="C5" r:id="rId4" display="https://hsquizbowl.org/db/tournaments/7370/" xr:uid="{40D1F2AD-20C0-644E-946F-1599053E8054}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{F35C47F0-70BB-DE4F-9B14-1657C13A4D43}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{25C8790F-46F2-6D45-B286-7DEBA4169B52}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{7FA883E6-2F16-A94B-8465-06774E05E09B}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{E7AFF273-7F98-D147-8366-92DBD6E1739B}"/>
+    <hyperlink ref="C7" r:id="rId5" xr:uid="{A07F658B-FFD4-724B-B692-623AA39BD09B}"/>
+    <hyperlink ref="C6" r:id="rId6" xr:uid="{92A0EC0A-9017-B346-ACDE-95149B8661EF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
-  <legacyDrawing r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
+  <legacyDrawing r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -2001,8 +3727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E3F142A-4698-834F-8261-DB2006E5DBFB}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="184" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="184" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20"/>
@@ -2023,16 +3749,16 @@
       <c r="A2" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="17" t="s">
-        <v>44</v>
+      <c r="B2" s="14" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="160" customHeight="1">
       <c r="A3" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="18" t="s">
-        <v>45</v>
+      <c r="B3" s="15" t="s">
+        <v>216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating prelims_data excel file for colab testing
I've been working with a prelims_data sheet I created after a tournament in Long Island, which populated a hypothetical prelims schedule for that tournament (I did not implement Cornerstone at that tournament). In the time that I've ported Cornerstone over to Colab, I've been using that file for testing. I'm overwriting the prelims_data.xlsx file here and then will directly pull data from github to colab for continued testing, instead of re-uploading the file each time.
</commit_message>
<xml_diff>
--- a/data input/prelims_data.xlsx
+++ b/data input/prelims_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/victorprieto/Desktop/code/cornerstone/data input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\z004ercu\Desktop\python\cornerstone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1642907F-100B-9A4D-82C3-3A881DB734E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9448B731-F64B-4990-94A5-8803A7733FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3380" yWindow="500" windowWidth="30220" windowHeight="19000" xr2:uid="{2114AE23-4723-3F48-88AE-F53CC59B0CBE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{2114AE23-4723-3F48-88AE-F53CC59B0CBE}"/>
   </bookViews>
   <sheets>
     <sheet name="tournament format" sheetId="6" r:id="rId1"/>
@@ -21,9 +21,6 @@
     <sheet name="QR codes" sheetId="5" r:id="rId6"/>
     <sheet name="text input" sheetId="4" r:id="rId7"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId8"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -32,8 +29,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -627,137 +628,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="tournament format"/>
-      <sheetName val="list of teams"/>
-      <sheetName val="team codes"/>
-      <sheetName val="group names"/>
-      <sheetName val="room assignments"/>
-      <sheetName val="QR codes"/>
-      <sheetName val="text input"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>Hunter B</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>Valley Stream S</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>North Babylon B</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5" t="str">
-            <v>Kings Park B</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6" t="str">
-            <v>Darien A</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7" t="str">
-            <v>Chenery</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8" t="str">
-            <v>High Tech C</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9" t="str">
-            <v>Kings Park C</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10" t="str">
-            <v>Island Trees</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11" t="str">
-            <v>North Babylon A</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12" t="str">
-            <v>Darien B</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="A13" t="str">
-            <v>High Tech B</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="A14" t="str">
-            <v>Hunter A</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="A15" t="str">
-            <v>Mepham B</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="A16" t="str">
-            <v>Kings Park D</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="A17" t="str">
-            <v>High Tech A</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="A18" t="str">
-            <v>Mepham A</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="A19" t="str">
-            <v>Woodland Reg.</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="A20" t="str">
-            <v>Port Jefferson</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="A21" t="str">
-            <v>Wilton</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="A22" t="str">
-            <v>Hunter C</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1059,11 +929,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39DE5B6E-5562-4B4B-9B01-3722A29F012F}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="20"/>
   <cols>
     <col min="1" max="1" width="42.33203125" customWidth="1"/>
     <col min="2" max="2" width="25.33203125" customWidth="1"/>
@@ -1161,7 +1031,7 @@
       <selection pane="bottomLeft" activeCell="C16" sqref="C16:C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="20"/>
   <cols>
     <col min="1" max="1" width="28.109375" style="3" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" style="3" customWidth="1"/>
@@ -1442,11 +1312,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7DB3BDA-97A0-7C48-BC5D-89202C03BA23}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="20"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
   </cols>
@@ -1461,7 +1331,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="18" t="str">
-        <f>'[1]list of teams'!A2</f>
+        <f>'list of teams'!A2</f>
         <v>Hunter B</v>
       </c>
       <c r="B2" s="19" t="s">
@@ -1470,7 +1340,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="18" t="str">
-        <f>'[1]list of teams'!A3</f>
+        <f>'list of teams'!A3</f>
         <v>Valley Stream S</v>
       </c>
       <c r="B3" s="19" t="s">
@@ -1479,7 +1349,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="18" t="str">
-        <f>'[1]list of teams'!A4</f>
+        <f>'list of teams'!A4</f>
         <v>North Babylon B</v>
       </c>
       <c r="B4" s="19" t="s">
@@ -1488,7 +1358,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="18" t="str">
-        <f>'[1]list of teams'!A5</f>
+        <f>'list of teams'!A5</f>
         <v>Kings Park B</v>
       </c>
       <c r="B5" s="19" t="s">
@@ -1497,7 +1367,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="18" t="str">
-        <f>'[1]list of teams'!A6</f>
+        <f>'list of teams'!A6</f>
         <v>Darien A</v>
       </c>
       <c r="B6" s="19" t="s">
@@ -1506,7 +1376,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="18" t="str">
-        <f>'[1]list of teams'!A7</f>
+        <f>'list of teams'!A7</f>
         <v>Chenery</v>
       </c>
       <c r="B7" s="19" t="s">
@@ -1515,7 +1385,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="18" t="str">
-        <f>'[1]list of teams'!A8</f>
+        <f>'list of teams'!A8</f>
         <v>High Tech C</v>
       </c>
       <c r="B8" s="19" t="s">
@@ -1524,7 +1394,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="18" t="str">
-        <f>'[1]list of teams'!A9</f>
+        <f>'list of teams'!A9</f>
         <v>Kings Park C</v>
       </c>
       <c r="B9" s="19" t="s">
@@ -1533,7 +1403,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="18" t="str">
-        <f>'[1]list of teams'!A10</f>
+        <f>'list of teams'!A10</f>
         <v>Island Trees</v>
       </c>
       <c r="B10" s="19" t="s">
@@ -1542,7 +1412,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="18" t="str">
-        <f>'[1]list of teams'!A11</f>
+        <f>'list of teams'!A11</f>
         <v>North Babylon A</v>
       </c>
       <c r="B11" s="19" t="s">
@@ -1551,7 +1421,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="18" t="str">
-        <f>'[1]list of teams'!A12</f>
+        <f>'list of teams'!A12</f>
         <v>Darien B</v>
       </c>
       <c r="B12" s="19" t="s">
@@ -1560,7 +1430,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="18" t="str">
-        <f>'[1]list of teams'!A13</f>
+        <f>'list of teams'!A13</f>
         <v>High Tech B</v>
       </c>
       <c r="B13" s="19" t="s">
@@ -1569,7 +1439,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="18" t="str">
-        <f>'[1]list of teams'!A14</f>
+        <f>'list of teams'!A14</f>
         <v>Hunter A</v>
       </c>
       <c r="B14" s="19" t="s">
@@ -1578,7 +1448,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="18" t="str">
-        <f>'[1]list of teams'!A15</f>
+        <f>'list of teams'!A15</f>
         <v>Mepham B</v>
       </c>
       <c r="B15" s="19" t="s">
@@ -1587,7 +1457,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="18" t="str">
-        <f>'[1]list of teams'!A16</f>
+        <f>'list of teams'!A16</f>
         <v>Kings Park D</v>
       </c>
       <c r="B16" s="19" t="s">
@@ -1596,7 +1466,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="18" t="str">
-        <f>'[1]list of teams'!A17</f>
+        <f>'list of teams'!A17</f>
         <v>High Tech A</v>
       </c>
       <c r="B17" s="19" t="s">
@@ -1605,7 +1475,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="18" t="str">
-        <f>'[1]list of teams'!A18</f>
+        <f>'list of teams'!A18</f>
         <v>Mepham A</v>
       </c>
       <c r="B18" s="19" t="s">
@@ -1614,7 +1484,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="18" t="str">
-        <f>'[1]list of teams'!A19</f>
+        <f>'list of teams'!A19</f>
         <v>Woodland Reg.</v>
       </c>
       <c r="B19" s="19" t="s">
@@ -1623,7 +1493,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="18" t="str">
-        <f>'[1]list of teams'!A20</f>
+        <f>'list of teams'!A20</f>
         <v>Port Jefferson</v>
       </c>
       <c r="B20" s="19" t="s">
@@ -1632,7 +1502,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="18" t="str">
-        <f>'[1]list of teams'!A21</f>
+        <f>'list of teams'!A21</f>
         <v>Wilton</v>
       </c>
       <c r="B21" s="19" t="s">
@@ -1641,7 +1511,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="18" t="str">
-        <f>'[1]list of teams'!A22</f>
+        <f>'list of teams'!A22</f>
         <v>Hunter C</v>
       </c>
       <c r="B22" s="19" t="s">
@@ -1650,6 +1520,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1661,7 +1532,7 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="20"/>
   <cols>
     <col min="1" max="1" width="19.21875" customWidth="1"/>
   </cols>
@@ -1723,7 +1594,7 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="20"/>
   <cols>
     <col min="1" max="1" width="12.44140625" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" customWidth="1"/>
@@ -1864,7 +1735,7 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="20"/>
   <cols>
     <col min="1" max="1" width="11.5546875" customWidth="1"/>
     <col min="2" max="2" width="21.109375" customWidth="1"/>
@@ -1994,7 +1865,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="20"/>
   <cols>
     <col min="1" max="1" width="32.33203125" customWidth="1"/>
     <col min="2" max="2" width="47.109375" customWidth="1"/>

</xml_diff>

<commit_message>
changed qr_toggle to Y in prelims data input
</commit_message>
<xml_diff>
--- a/data input/prelims_data.xlsx
+++ b/data input/prelims_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\z004ercu\Desktop\python\cornerstone\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\z004ercu\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9448B731-F64B-4990-94A5-8803A7733FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A50ECA-C231-4F1E-BF38-9F6303EF1BF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{2114AE23-4723-3F48-88AE-F53CC59B0CBE}"/>
+    <workbookView xWindow="57490" yWindow="-110" windowWidth="29020" windowHeight="15820" xr2:uid="{2114AE23-4723-3F48-88AE-F53CC59B0CBE}"/>
   </bookViews>
   <sheets>
     <sheet name="tournament format" sheetId="6" r:id="rId1"/>
@@ -33,8 +33,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -65,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="96">
   <si>
     <t>Team</t>
   </si>
@@ -353,9 +351,6 @@
   </si>
   <si>
     <t>Room 242</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
 </sst>
 </file>
@@ -929,7 +924,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39DE5B6E-5562-4B4B-9B01-3722A29F012F}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -989,7 +984,7 @@
         <v>17</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>96</v>
+        <v>37</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>32</v>
@@ -1312,7 +1307,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7DB3BDA-97A0-7C48-BC5D-89202C03BA23}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>

</xml_diff>